<commit_message>
Thesis is updated. Inertial support limits are investigated.
</commit_message>
<xml_diff>
--- a/Thesis/Matlab Codes/World Renewable Capacity and Production/World Renewable Capacity.xlsx
+++ b/Thesis/Matlab Codes/World Renewable Capacity and Production/World Renewable Capacity.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Capacity" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
-    <sheet name="Production" sheetId="2" r:id="rId3"/>
-    <sheet name="Productionpercap" sheetId="3" r:id="rId4"/>
+    <sheet name="2017-2018" sheetId="4" r:id="rId1"/>
+    <sheet name="2018" sheetId="5" r:id="rId2"/>
+    <sheet name="2017" sheetId="1" r:id="rId3"/>
+    <sheet name="Production" sheetId="2" r:id="rId4"/>
+    <sheet name="Productionpercap" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="24">
   <si>
     <t>Country</t>
   </si>
@@ -83,6 +84,18 @@
   <si>
     <t>Rus.Fed.</t>
   </si>
+  <si>
+    <t>Capacity(GW)</t>
+  </si>
+  <si>
+    <t>Addition in 2017</t>
+  </si>
+  <si>
+    <t>2018 Report Cap</t>
+  </si>
+  <si>
+    <t>2017 Report Cap</t>
+  </si>
 </sst>
 </file>
 
@@ -125,9 +138,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -146,6 +163,438 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.3419878270611855E-2"/>
+          <c:y val="4.1467304625199361E-2"/>
+          <c:w val="0.89899419047439211"/>
+          <c:h val="0.77849229199139736"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>MW</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2017'!$B$2:$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Germany</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>India</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Japan</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Rus.Fed.</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Turkey</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Sweeden</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2017'!$D$2:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>545.91600000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>214.76599999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>122.95099999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104.70399999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.516999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.748000000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75.125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>51.07</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>47.954000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44.665999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>34.466999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33.515999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32.744</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-32A0-427F-851E-F6BDC2E2768F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="253407760"/>
+        <c:axId val="253414000"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="253407760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="tr-TR" sz="1200"/>
+                  <a:t>Countries</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="tr-TR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="tr-TR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="253414000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="253414000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="tr-TR" sz="1200"/>
+                  <a:t>MW</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="tr-TR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="tr-TR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="253407760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="tr-TR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -184,7 +633,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Capacity!$B$2:$B$16</c:f>
+              <c:f>'2018'!$B$2:$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -200,19 +649,19 @@
                   <c:v>Germany</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>India</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Canada</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>India</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Japan</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Rus.Fed.</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Italy</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Spain</c:v>
@@ -221,10 +670,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Turkey</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Norway</c:v>
@@ -237,7 +686,377 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Capacity!$D$2:$D$15</c:f>
+              <c:f>'2018'!$D$2:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>618.803</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>229.91300000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128.29300000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>113.05800000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>106.282</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>98.697000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>82.695999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51.951000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>51.779000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>47.988999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46.677999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40.789000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>38.725000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>33.283000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-30B6-4053-9121-27EE73B8A112}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="253407760"/>
+        <c:axId val="253414000"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="253407760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="tr-TR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="253414000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="253414000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="tr-TR" sz="1200">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>MW</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="tr-TR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="tr-TR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="253407760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="tr-TR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>MW</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2017'!$B$2:$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Germany</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>India</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Japan</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Rus.Fed.</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Turkey</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Sweeden</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2017'!$D$2:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -406,7 +1225,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -516,441 +1334,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="8.3419878270611855E-2"/>
-          <c:y val="4.1467304625199361E-2"/>
-          <c:w val="0.89899419047439211"/>
-          <c:h val="0.77849229199139736"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>MW</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Capacity!$B$2:$B$16</c:f>
-              <c:strCache>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>USA</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Brazil</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Germany</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Canada</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>India</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Japan</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Rus.Fed.</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Spain</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>France</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Turkey</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>UK</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Sweeden</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Capacity!$D$2:$D$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>545.91600000000005</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>214.76599999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>122.95099999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>104.70399999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>97.516999999999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>90.748000000000005</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>75.125</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>51.35</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>51.07</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>47.954000000000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44.665999999999997</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>34.466999999999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>33.515999999999998</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>32.744</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-32A0-427F-851E-F6BDC2E2768F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="253407760"/>
-        <c:axId val="253414000"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="253407760"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="tr-TR" sz="1200"/>
-                  <a:t>Countries</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="tr-TR"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="253414000"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="253414000"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="tr-TR" sz="1200"/>
-                  <a:t>MW</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="tr-TR"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="253407760"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="tr-TR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1322,7 +1706,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1337,6 +1721,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1404,7 +1789,7 @@
                   <c:v>Brazil</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Russian Fed</c:v>
+                  <c:v>Rus. Fed.</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>USA</c:v>
@@ -1824,6 +2209,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3836,7 +4261,584 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>257176</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3871,44 +4873,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3945,7 +4910,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4243,10 +5208,260 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B27:D44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="str">
+        <f>'2018'!B30</f>
+        <v>China</v>
+      </c>
+      <c r="C28" s="3">
+        <f>'2017'!D30</f>
+        <v>545.91600000000005</v>
+      </c>
+      <c r="D28">
+        <f>'2018'!D30</f>
+        <v>618.803</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="str">
+        <f>'2018'!B42</f>
+        <v>USA</v>
+      </c>
+      <c r="C29" s="3">
+        <f>'2017'!D42</f>
+        <v>214.76599999999999</v>
+      </c>
+      <c r="D29">
+        <f>'2018'!D42</f>
+        <v>229.91300000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="str">
+        <f>'2018'!B28</f>
+        <v>Brazil</v>
+      </c>
+      <c r="C30" s="3">
+        <f>'2017'!D28</f>
+        <v>122.95099999999999</v>
+      </c>
+      <c r="D30">
+        <f>'2018'!D28</f>
+        <v>128.29300000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="str">
+        <f>'2018'!B32</f>
+        <v>Germany</v>
+      </c>
+      <c r="C31" s="3">
+        <f>'2017'!D32</f>
+        <v>104.70399999999999</v>
+      </c>
+      <c r="D31">
+        <f>'2018'!D32</f>
+        <v>113.05800000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="str">
+        <f>'2018'!B33</f>
+        <v>India</v>
+      </c>
+      <c r="C32" s="3">
+        <f>'2017'!D33</f>
+        <v>90.748000000000005</v>
+      </c>
+      <c r="D32">
+        <f>'2018'!D33</f>
+        <v>106.282</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="str">
+        <f>'2018'!B29</f>
+        <v>Canada</v>
+      </c>
+      <c r="C33" s="3">
+        <f>'2017'!D29</f>
+        <v>97.516999999999996</v>
+      </c>
+      <c r="D33">
+        <f>'2018'!D29</f>
+        <v>98.697000000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="str">
+        <f>'2018'!B35</f>
+        <v>Japan</v>
+      </c>
+      <c r="C34" s="3">
+        <f>'2017'!D35</f>
+        <v>75.125</v>
+      </c>
+      <c r="D34">
+        <f>'2018'!D35</f>
+        <v>82.695999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="str">
+        <f>'2018'!B34</f>
+        <v>Italy</v>
+      </c>
+      <c r="C35" s="3">
+        <f>'2017'!D34</f>
+        <v>51.07</v>
+      </c>
+      <c r="D35">
+        <f>'2018'!D34</f>
+        <v>51.951000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="str">
+        <f>'2018'!B37</f>
+        <v>Rus.Fed.</v>
+      </c>
+      <c r="C36" s="3">
+        <f>'2017'!D37</f>
+        <v>51.35</v>
+      </c>
+      <c r="D36">
+        <f>'2018'!D37</f>
+        <v>51.779000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="str">
+        <f>'2018'!B38</f>
+        <v>Spain</v>
+      </c>
+      <c r="C37" s="3">
+        <f>'2017'!D38</f>
+        <v>47.954000000000001</v>
+      </c>
+      <c r="D37">
+        <f>'2018'!D38</f>
+        <v>47.988999999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="str">
+        <f>'2018'!B31</f>
+        <v>France</v>
+      </c>
+      <c r="C38" s="3">
+        <f>'2017'!D31</f>
+        <v>44.665999999999997</v>
+      </c>
+      <c r="D38">
+        <f>'2018'!D31</f>
+        <v>46.677999999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="str">
+        <f>'2018'!B41</f>
+        <v>UK</v>
+      </c>
+      <c r="C39" s="3">
+        <f>'2017'!D41</f>
+        <v>33.515999999999998</v>
+      </c>
+      <c r="D39">
+        <f>'2018'!D41</f>
+        <v>40.789000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="str">
+        <f>'2018'!B40</f>
+        <v>Turkey</v>
+      </c>
+      <c r="C40" s="3">
+        <f>'2017'!D40</f>
+        <v>34.466999999999999</v>
+      </c>
+      <c r="D40">
+        <f>'2018'!D40</f>
+        <v>38.725000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="str">
+        <f>'2018'!B36</f>
+        <v>Norway</v>
+      </c>
+      <c r="C41" s="3">
+        <f>'2017'!D36</f>
+        <v>32.744</v>
+      </c>
+      <c r="D41">
+        <f>'2018'!D36</f>
+        <v>33.283000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="str">
+        <f>'2018'!B39</f>
+        <v>Sweeden</v>
+      </c>
+      <c r="C42" s="3">
+        <f>'2017'!D39</f>
+        <v>27.876999999999999</v>
+      </c>
+      <c r="D42">
+        <f>'2018'!D39</f>
+        <v>28.216999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="3"/>
+    </row>
+  </sheetData>
+  <sortState ref="B28:D42">
+    <sortCondition descending="1" ref="D28:D42"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4268,6 +5483,421 @@
         <v>2</v>
       </c>
       <c r="C2">
+        <v>618803</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D16" si="0">C2/1000</f>
+        <v>618.803</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>229913</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>229.91300000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>128293</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>128.29300000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>113058</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>113.05800000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>106282</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>106.282</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>98697</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>98.697000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>82696</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>82.695999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>51951</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>51.951000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>51779</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>51.779000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>47989</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>47.988999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>46678</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>46.677999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>40789</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>40.789000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>38725</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>38.725000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>33283</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>33.283000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>28217</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>28.216999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f>SUM(D2:D5)</f>
+        <v>1090.067</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>2179.0990000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <v>128293</v>
+      </c>
+      <c r="D28">
+        <f t="shared" ref="D28:D42" si="1">C28/1000</f>
+        <v>128.29300000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>98697</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>98.697000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>618803</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>618.803</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31">
+        <v>46678</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>46.677999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>113058</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>113.05800000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>106282</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>106.282</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34">
+        <v>51951</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>51.951000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>82696</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>82.695999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <v>33283</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>33.283000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37">
+        <v>51779</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>51.779000000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38">
+        <v>47989</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>47.988999999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39">
+        <v>28217</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>28.216999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40">
+        <v>38725</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>38.725000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41">
+        <v>40789</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>40.789000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42">
+        <v>229913</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>229.91300000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B28:D42">
+    <sortCondition ref="B28:B42"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
         <v>545916</v>
       </c>
       <c r="D2">
@@ -4443,64 +6073,589 @@
         <v>27.876999999999999</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D18">
         <f>SUM(D2:D5)</f>
         <v>988.33699999999999</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D20">
         <f>SUM(D2:D16)</f>
         <v>1575.3709999999999</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>15</v>
       </c>
       <c r="C28">
         <v>122951</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <f t="shared" ref="D28:D42" si="1">C28/1000</f>
+        <v>122.95099999999999</v>
+      </c>
+      <c r="E28">
+        <f>F28/1000</f>
+        <v>5.3419999999999996</v>
+      </c>
+      <c r="F28">
+        <f>'2018'!C28-'2017'!C28</f>
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>14</v>
       </c>
       <c r="C29">
         <v>97517</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>97.516999999999996</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ref="E29:E42" si="2">F29/1000</f>
+        <v>1.18</v>
+      </c>
+      <c r="F29">
+        <f>'2018'!C29-'2017'!C29</f>
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>2</v>
       </c>
       <c r="C30">
         <v>545916</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>545.91600000000005</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>72.887</v>
+      </c>
+      <c r="F30">
+        <f>'2018'!C30-'2017'!C30</f>
+        <v>72887</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>7</v>
       </c>
       <c r="C31">
         <v>44666</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>44.665999999999997</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>2.012</v>
+      </c>
+      <c r="F31">
+        <f>'2018'!C31-'2017'!C31</f>
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>8</v>
       </c>
       <c r="C32">
         <v>104704</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>104.70399999999999</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>8.3539999999999992</v>
+      </c>
+      <c r="F32">
+        <f>'2018'!C32-'2017'!C32</f>
+        <v>8354</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>90748</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>90.748000000000005</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>15.534000000000001</v>
+      </c>
+      <c r="F33">
+        <f>'2018'!C33-'2017'!C33</f>
+        <v>15534</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34">
+        <v>51070</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>51.07</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="F34">
+        <f>'2018'!C34-'2017'!C34</f>
+        <v>881</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>75125</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>75.125</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>7.5709999999999997</v>
+      </c>
+      <c r="F35">
+        <f>'2018'!C35-'2017'!C35</f>
+        <v>7571</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <v>32744</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>32.744</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="F36">
+        <f>'2018'!C36-'2017'!C36</f>
+        <v>539</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37">
+        <v>51350</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>51.35</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="F37">
+        <f>'2018'!C37-'2017'!C37</f>
+        <v>429</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38">
+        <v>47954</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>47.954000000000001</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F38">
+        <f>'2018'!C38-'2017'!C38</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39">
+        <v>27877</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>27.876999999999999</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>0.34</v>
+      </c>
+      <c r="F39">
+        <f>'2018'!C39-'2017'!C39</f>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40">
+        <v>34467</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>34.466999999999999</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>4.258</v>
+      </c>
+      <c r="F40">
+        <f>'2018'!C40-'2017'!C40</f>
+        <v>4258</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41">
+        <v>33516</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>33.515999999999998</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>7.2729999999999997</v>
+      </c>
+      <c r="F41">
+        <f>'2018'!C41-'2017'!C41</f>
+        <v>7273</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42">
+        <v>214766</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>214.76599999999999</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>15.147</v>
+      </c>
+      <c r="F42">
+        <f>'2018'!C42-'2017'!C42</f>
+        <v>15147</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B28:D42">
+    <sortCondition ref="B28:B42"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1371762</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D16" si="0">C2/1000</f>
+        <v>1371.7619999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>562451</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>562.45100000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>430490</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>430.49</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>422553</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>422.553</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>210493</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>210.49299999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>187005</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>187.005</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>168617</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>168.61699999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>166751</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>166.751</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>140639</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>140.63900000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>108917</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>108.917</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>102443</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>102.443</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>97089</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>97.088999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>89358</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>89.358000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>83568</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>83.567999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>82943</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>82.942999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <v>430490</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>422553</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>1371762</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31">
+        <v>89358</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>187005</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
@@ -4508,7 +6663,7 @@
         <v>3</v>
       </c>
       <c r="C33">
-        <v>90748</v>
+        <v>210493</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
@@ -4516,7 +6671,7 @@
         <v>9</v>
       </c>
       <c r="C34">
-        <v>51070</v>
+        <v>108917</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
@@ -4524,7 +6679,7 @@
         <v>4</v>
       </c>
       <c r="C35">
-        <v>75125</v>
+        <v>166751</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
@@ -4532,7 +6687,7 @@
         <v>10</v>
       </c>
       <c r="C36">
-        <v>32744</v>
+        <v>140639</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
@@ -4540,7 +6695,7 @@
         <v>5</v>
       </c>
       <c r="C37">
-        <v>51350</v>
+        <v>168617</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
@@ -4548,7 +6703,7 @@
         <v>11</v>
       </c>
       <c r="C38">
-        <v>47954</v>
+        <v>97089</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
@@ -4556,7 +6711,7 @@
         <v>12</v>
       </c>
       <c r="C39">
-        <v>27877</v>
+        <v>102443</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
@@ -4564,7 +6719,7 @@
         <v>6</v>
       </c>
       <c r="C40">
-        <v>34467</v>
+        <v>83568</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
@@ -4572,7 +6727,7 @@
         <v>13</v>
       </c>
       <c r="C41">
-        <v>33516</v>
+        <v>82943</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
@@ -4580,7 +6735,7 @@
         <v>16</v>
       </c>
       <c r="C42">
-        <v>214766</v>
+        <v>562451</v>
       </c>
     </row>
   </sheetData>
@@ -4593,366 +6748,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D42"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>1371762</v>
-      </c>
-      <c r="D2">
-        <f t="shared" ref="D2:D16" si="0">C2/1000</f>
-        <v>1371.7619999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3">
-        <v>562451</v>
-      </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
-        <v>562.45100000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4">
-        <v>430490</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>430.49</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
-        <v>422553</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>422.553</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>210493</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>210.49299999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>187005</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>187.005</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8">
-        <v>168617</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>168.61699999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>166751</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>166.751</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10">
-        <v>140639</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>140.63900000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11">
-        <v>108917</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>108.917</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12">
-        <v>102443</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>102.443</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13">
-        <v>97089</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>97.088999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14">
-        <v>89358</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>89.358000000000004</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15">
-        <v>83568</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>83.567999999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16">
-        <v>82943</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>82.942999999999998</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28">
-        <v>430490</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29">
-        <v>422553</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30">
-        <v>1371762</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31">
-        <v>89358</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32">
-        <v>187005</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33">
-        <v>210493</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34">
-        <v>108917</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35">
-        <v>166751</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36">
-        <v>140639</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37">
-        <v>168617</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38">
-        <v>97089</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39">
-        <v>102443</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40">
-        <v>83568</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41">
-        <v>82943</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42">
-        <v>562451</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="B28:C42">
-    <sortCondition ref="B28:B42"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4974,7 +6775,7 @@
         <v>15</v>
       </c>
       <c r="C2">
-        <f>Production!C28/Capacity!C28</f>
+        <f>Production!C28/'2017'!C28</f>
         <v>3.5013135314068204</v>
       </c>
     </row>
@@ -4983,7 +6784,7 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <f>Production!C29/Capacity!C29</f>
+        <f>Production!C29/'2017'!C29</f>
         <v>4.3331214044730659</v>
       </c>
     </row>
@@ -4992,7 +6793,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <f>Production!C30/Capacity!C30</f>
+        <f>Production!C30/'2017'!C30</f>
         <v>2.5127711955685492</v>
       </c>
     </row>
@@ -5001,7 +6802,7 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <f>Production!C31/Capacity!C31</f>
+        <f>Production!C31/'2017'!C31</f>
         <v>2.0005820982402724</v>
       </c>
     </row>
@@ -5010,7 +6811,7 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <f>Production!C32/Capacity!C32</f>
+        <f>Production!C32/'2017'!C32</f>
         <v>1.7860349174816625</v>
       </c>
     </row>
@@ -5019,7 +6820,7 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <f>Production!C33/Capacity!C33</f>
+        <f>Production!C33/'2017'!C33</f>
         <v>2.3195332128531758</v>
       </c>
     </row>
@@ -5028,7 +6829,7 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <f>Production!C34/Capacity!C34</f>
+        <f>Production!C34/'2017'!C34</f>
         <v>2.1327002153906403</v>
       </c>
     </row>
@@ -5037,7 +6838,7 @@
         <v>4</v>
       </c>
       <c r="C9">
-        <f>Production!C35/Capacity!C35</f>
+        <f>Production!C35/'2017'!C35</f>
         <v>2.2196472545757073</v>
       </c>
     </row>
@@ -5046,7 +6847,7 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <f>Production!C36/Capacity!C36</f>
+        <f>Production!C36/'2017'!C36</f>
         <v>4.2951075006107988</v>
       </c>
     </row>
@@ -5055,7 +6856,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <f>Production!C37/Capacity!C37</f>
+        <f>Production!C37/'2017'!C37</f>
         <v>3.2836806231742939</v>
       </c>
     </row>
@@ -5064,7 +6865,7 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <f>Production!C38/Capacity!C38</f>
+        <f>Production!C38/'2017'!C38</f>
         <v>2.024627768277933</v>
       </c>
     </row>
@@ -5073,7 +6874,7 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <f>Production!C39/Capacity!C39</f>
+        <f>Production!C39/'2017'!C39</f>
         <v>3.6748215374681639</v>
       </c>
     </row>
@@ -5082,7 +6883,7 @@
         <v>6</v>
       </c>
       <c r="C14">
-        <f>Production!C40/Capacity!C40</f>
+        <f>Production!C40/'2017'!C40</f>
         <v>2.4245800330751153</v>
       </c>
     </row>
@@ -5091,7 +6892,7 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <f>Production!C41/Capacity!C41</f>
+        <f>Production!C41/'2017'!C41</f>
         <v>2.4747284878863827</v>
       </c>
     </row>
@@ -5100,7 +6901,7 @@
         <v>16</v>
       </c>
       <c r="C16">
-        <f>Production!C42/Capacity!C42</f>
+        <f>Production!C42/'2017'!C42</f>
         <v>2.61890150209996</v>
       </c>
     </row>
@@ -5146,7 +6947,7 @@
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C25">
         <v>3.2836806231742939</v>

</xml_diff>

<commit_message>
Chapter 1 is updated.
</commit_message>
<xml_diff>
--- a/Thesis/Matlab Codes/World Renewable Capacity and Production/World Renewable Capacity.xlsx
+++ b/Thesis/Matlab Codes/World Renewable Capacity and Production/World Renewable Capacity.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="2017-2018" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="25">
   <si>
     <t>Country</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>2017 Report Cap</t>
+  </si>
+  <si>
+    <t>Sweden</t>
   </si>
 </sst>
 </file>
@@ -679,7 +682,7 @@
                   <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Sweeden</c:v>
+                  <c:v>Sweden</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1467,7 +1470,7 @@
                   <c:v>Italy</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Sweeden</c:v>
+                  <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Spain</c:v>
@@ -1721,7 +1724,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1783,7 +1785,7 @@
                   <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Sweeden</c:v>
+                  <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Brazil</c:v>
@@ -5210,8 +5212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B27:D44"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5430,7 +5432,7 @@
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="str">
         <f>'2018'!B39</f>
-        <v>Sweeden</v>
+        <v>Sweden</v>
       </c>
       <c r="C42" s="3">
         <f>'2017'!D39</f>
@@ -5460,8 +5462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D42"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5648,7 +5650,7 @@
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C16">
         <v>28217</v>
@@ -5814,7 +5816,7 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C39">
         <v>28217</v>
@@ -6413,8 +6415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6552,7 +6554,7 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C12">
         <v>102443</v>
@@ -6708,7 +6710,7 @@
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C39">
         <v>102443</v>
@@ -6752,8 +6754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6871,7 +6873,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C13">
         <f>Production!C39/'2017'!C39</f>
@@ -6931,7 +6933,7 @@
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C23">
         <v>3.6748215374681639</v>

</xml_diff>